<commit_message>
export data from excel
</commit_message>
<xml_diff>
--- a/src/public/sites.xlsx
+++ b/src/public/sites.xlsx
@@ -20,12 +20,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t xml:space="preserve">sites</t>
+  </si>
+  <si>
+    <t xml:space="preserve">send</t>
+  </si>
   <si>
     <t xml:space="preserve">https://automatedconversions.com/</t>
   </si>
   <si>
+    <t xml:space="preserve">true</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://www.workmatix.com/digital-marketing-consulting-services/paid-search-management/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">falsy</t>
   </si>
 </sst>
 </file>
@@ -122,13 +134,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="75.07"/>
   </cols>
@@ -137,10 +149,24 @@
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>